<commit_message>
added is and kr
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SjobergD\GitHub\gtsummary-translation-gif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A75B8D-5FDB-47F6-8F65-6773771AE5C2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4577BF89-EC48-429D-8806-E3435B7EDA8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{0CF341BA-DD9F-4680-99DA-1DA4026995D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{0CF341BA-DD9F-4680-99DA-1DA4026995D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="109">
   <si>
     <t>zh-tw</t>
   </si>
@@ -313,6 +313,51 @@
   </si>
   <si>
     <t>Portuguese</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>Icelandic</t>
+  </si>
+  <si>
+    <t>Íslenska</t>
+  </si>
+  <si>
+    <t>Lyfjameðferð</t>
+  </si>
+  <si>
+    <t>Geislameðferð</t>
+  </si>
+  <si>
+    <t>Aldur</t>
+  </si>
+  <si>
+    <t>Æxlisstig</t>
+  </si>
+  <si>
+    <t>kr</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>한국어</t>
+  </si>
+  <si>
+    <t>방사선 요법</t>
+  </si>
+  <si>
+    <t>나이</t>
+  </si>
+  <si>
+    <t>농종 등급</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/c/ce/Flag_of_Iceland.svg/1280px-Flag_of_Iceland.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/0/09/Flag_of_South_Korea.svg/1280px-Flag_of_South_Korea.svg.png</t>
   </si>
 </sst>
 </file>
@@ -357,9 +402,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -675,13 +723,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479039AE-01F2-4E76-BADA-2E4CABC84037}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,9 +742,10 @@
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -733,8 +782,14 @@
       <c r="L1" t="s">
         <v>84</v>
       </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -771,8 +826,14 @@
       <c r="L2" t="s">
         <v>85</v>
       </c>
+      <c r="M2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N2" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -809,8 +870,14 @@
       <c r="L3" t="s">
         <v>86</v>
       </c>
+      <c r="M3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N3" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -847,8 +914,14 @@
       <c r="L4" t="s">
         <v>87</v>
       </c>
+      <c r="M4" t="s">
+        <v>97</v>
+      </c>
+      <c r="N4" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -885,8 +958,14 @@
       <c r="L5" t="s">
         <v>88</v>
       </c>
+      <c r="M5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N5" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -923,8 +1002,14 @@
       <c r="L6" t="s">
         <v>89</v>
       </c>
+      <c r="M6" t="s">
+        <v>99</v>
+      </c>
+      <c r="N6" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -961,8 +1046,14 @@
       <c r="L7" t="s">
         <v>90</v>
       </c>
+      <c r="M7" t="s">
+        <v>100</v>
+      </c>
+      <c r="N7" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -999,8 +1090,14 @@
       <c r="L8" t="s">
         <v>9</v>
       </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1037,8 +1134,14 @@
       <c r="L9" t="s">
         <v>10</v>
       </c>
+      <c r="M9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1075,8 +1178,14 @@
       <c r="L10" t="s">
         <v>11</v>
       </c>
+      <c r="M10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1112,6 +1221,12 @@
       </c>
       <c r="L11" t="s">
         <v>91</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1121,8 +1236,10 @@
     <hyperlink ref="D11" r:id="rId3" xr:uid="{01DD4385-2BBA-44FD-96EE-7BF5547E6AC4}"/>
     <hyperlink ref="E11" r:id="rId4" xr:uid="{5C0FA8A3-4498-4518-8DEF-D02C2D14579E}"/>
     <hyperlink ref="H11" r:id="rId5" xr:uid="{48982109-33C4-478B-B7D5-5A4ABE8CC31D}"/>
+    <hyperlink ref="N11" r:id="rId6" xr:uid="{FD6FCF86-34ED-402F-83B8-DC2D22786984}"/>
+    <hyperlink ref="M11" r:id="rId7" xr:uid="{7410B219-1570-452D-A494-E355A2DFFDAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>